<commit_message>
To many changes to spec here. Look at the changelist.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_props.xlsx
+++ b/data/guitar_strings_props.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ43" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ45" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ46" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ44" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ45FF" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ46FF" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="EJ43" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="EJ45" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="EJ46" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="EJ44" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="EJ45FF" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="EJ46FF" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Numerous typos fixed; deleted obsolete code
</commit_message>
<xml_diff>
--- a/data/guitar_strings_props.xlsx
+++ b/data/guitar_strings_props.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="EJ43" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="EJ45" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="EJ46" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="EJ44" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="EJ45FF" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="EJ46FF" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ43" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ45" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ46" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ44" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ45FF" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EJ46FF" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>